<commit_message>
implemented parallel executio of scenarios using pico cotainer.
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\MyGitFrameWork\BDD_Selenium_TestNG_Maven_CucumberReporting\src\test\resources\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15210" windowHeight="2760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="4575"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <customWorkbookViews>
     <customWorkbookView name="Admin - Personal View" guid="{338E119F-9ECD-468B-8CFF-D14A5168FE1D}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1616" windowHeight="876" activeSheetId="1"/>
   </customWorkbookViews>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -35,13 +31,22 @@
     <t>user</t>
   </si>
   <si>
-    <t>user0</t>
-  </si>
-  <si>
     <t>demo</t>
   </si>
   <si>
     <t>john</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>user4</t>
   </si>
 </sst>
 </file>
@@ -94,76 +99,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{86B65319-CAB9-4E3B-B536-F841FE5B90B3}" diskRevisions="1" revisionId="2" version="2">
-  <header guid="{4F7A7580-A11F-4516-BCB1-91E03E75B11F}" dateTime="2019-03-26T16:49:55" maxSheetId="4" userName="Admin" r:id="rId1">
-    <sheetIdMap count="3">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{86B65319-CAB9-4E3B-B536-F841FE5B90B3}" dateTime="2019-03-26T17:30:47" maxSheetId="4" userName="Admin" r:id="rId2" minRId="1" maxRId="2">
-    <sheetIdMap count="3">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-    </sheetIdMap>
-  </header>
-</headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rrc rId="1" sId="1" ref="A3:XFD3" action="deleteRow">
-    <rfmt sheetId="1" xfDxf="1" sqref="A3:XFD3" start="0" length="0"/>
-    <rcc rId="0" sId="1">
-      <nc r="A3" t="inlineStr">
-        <is>
-          <t>user0</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="1">
-      <nc r="B3" t="inlineStr">
-        <is>
-          <t>Alex</t>
-        </is>
-      </nc>
-    </rcc>
-    <rcc rId="0" sId="1">
-      <nc r="C3" t="inlineStr">
-        <is>
-          <t>demo</t>
-        </is>
-      </nc>
-    </rcc>
-  </rrc>
-  <rcc rId="2" sId="1">
-    <oc r="B2" t="inlineStr">
-      <is>
-        <t>Alex</t>
-      </is>
-    </oc>
-    <nc r="B2" t="inlineStr">
-      <is>
-        <t>john</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{86B65319-CAB9-4E3B-B536-F841FE5B90B3}" name="Admin" id="-949691630" dateTime="2019-03-26T16:49:55"/>
-</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -453,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,13 +409,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>